<commit_message>
new pars , shape coeff function, new data
 new pars , shape coeff function, new data
</commit_message>
<xml_diff>
--- a/Jones2009_Table3.3.xlsx
+++ b/Jones2009_Table3.3.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annaortega/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nina\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B896CB00-8AB1-DE4F-8F68-491EEE2F165E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976786BC-EB1F-4386-8850-8F6E961E4172}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8790" tabRatio="320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jones2009_3.3" sheetId="1" r:id="rId1"/>
+    <sheet name="Jones2009_3.1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Jones2009_3.3!$A$2:$F$48</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="148">
   <si>
     <t>this study</t>
   </si>
@@ -68,6 +69,429 @@
   </si>
   <si>
     <t>Table 3.2 SCL and mass-at-age of individual turtles raised in captivity. These data were used in figures 3.2 &amp; 3.3 to produce the length-mass relationships (when mass given) and the growth functions (length-at-age data).</t>
+  </si>
+  <si>
+    <t>Table 3.3. wild turtles</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Am.Samoa</t>
+  </si>
+  <si>
+    <t>Ceylon,India</t>
+  </si>
+  <si>
+    <t>MTN(1996)</t>
+  </si>
+  <si>
+    <t>J.Wyneken (pers.comm)</t>
+  </si>
+  <si>
+    <t>NOAA (NMFS/PIFSC)</t>
+  </si>
+  <si>
+    <t>MTN(2004)</t>
+  </si>
+  <si>
+    <t>M.Conti (pers.comm)</t>
+  </si>
+  <si>
+    <t>Florida,USA</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Hawaii,USA</t>
+  </si>
+  <si>
+    <t>W.Australia</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">DATA USED FOR MODEL PARAMETER ESTIMATION: Based on the  qualitative (visual) data analysis, we've decided to  use data from Tables 3.2 and 3.3, combined with data from Zug et al  (1986) presented in figure 3.2. This meant NOT using data in Table 3.1 (means of all individuals throughout growth in captivity -- means may be skewed, and some individuals over-represented in the dataset --eg, last 10 or so red stars in figures below all belong to the same individual). Instead, we use 1-point-per-turtle (presented in Table 3.2) for growth in captivity, combined with data from other studies of captive growth. 
+This also meant </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">removing </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> some data from tL1 dataset (original D.coriacea entry) and reorganizing it, to reflect correctly wild vs captive individuals</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">% SCL = straight carapace length  </t>
+  </si>
+  <si>
+    <t>tLW_Jone = [ ... (time since birth (yr) SCL (cm) weight (kg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.003 6.31  0.046 % N = 20 turtles </t>
+  </si>
+  <si>
+    <t>0.01  6.53  0.05 % (N=19)</t>
+  </si>
+  <si>
+    <t>0.03  7.22  0.06 % N=20</t>
+  </si>
+  <si>
+    <t>0.05  7.81  0.08</t>
+  </si>
+  <si>
+    <t>0.07  8.31  0.10</t>
+  </si>
+  <si>
+    <t>0.08  8.91  0.12</t>
+  </si>
+  <si>
+    <t>0.10  9.59  0.15</t>
+  </si>
+  <si>
+    <t>0.12 10.28  0.18</t>
+  </si>
+  <si>
+    <t>0.14 10.76  0.21</t>
+  </si>
+  <si>
+    <t>0.16 11.33  0.24</t>
+  </si>
+  <si>
+    <t>0.18 12.10  0.28 % N = 16</t>
+  </si>
+  <si>
+    <t>0.20 12.77  0.32 % N = 19</t>
+  </si>
+  <si>
+    <t>0.22 13.20  0.37 % N = 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.24 13.64  0.41 </t>
+  </si>
+  <si>
+    <t>0.26 14.35  0.45</t>
+  </si>
+  <si>
+    <t>0.28 14.92  0.51</t>
+  </si>
+  <si>
+    <t>0.30 15.49  0.56</t>
+  </si>
+  <si>
+    <t>0.32 16.04  0.62</t>
+  </si>
+  <si>
+    <t>0.33 16.49  0.68 % N = 16</t>
+  </si>
+  <si>
+    <t>0.35 17.50  0.82 % N = 12</t>
+  </si>
+  <si>
+    <t>0.37  18.23 0.91 % N = 10</t>
+  </si>
+  <si>
+    <t>0.39 18.88  1.01</t>
+  </si>
+  <si>
+    <t>0.41 19.41  1.10</t>
+  </si>
+  <si>
+    <t>0.43 20.10  1.21</t>
+  </si>
+  <si>
+    <t>0.45 20.55  1.28</t>
+  </si>
+  <si>
+    <t>0.47 21.19  1.39</t>
+  </si>
+  <si>
+    <t>0.49 22.04  1.51</t>
+  </si>
+  <si>
+    <t>0.51 22.61  1.68</t>
+  </si>
+  <si>
+    <t>0.53 23.68  1.87 % N = 9</t>
+  </si>
+  <si>
+    <t>0.55 24.40  2.03</t>
+  </si>
+  <si>
+    <t>0.56 25.14  2.28</t>
+  </si>
+  <si>
+    <t>0.58 25.82  2.40</t>
+  </si>
+  <si>
+    <t>0.60 26.27  2.63</t>
+  </si>
+  <si>
+    <t>0.62 27.57  2.81 % N = 7</t>
+  </si>
+  <si>
+    <t>0.64 28.10  3.03</t>
+  </si>
+  <si>
+    <t>0.66 28.61  3.20</t>
+  </si>
+  <si>
+    <t>0.68 29.31  3.47</t>
+  </si>
+  <si>
+    <t>0.70 30.21  3.77 % N = 6</t>
+  </si>
+  <si>
+    <t>0.72 30.92  4.15</t>
+  </si>
+  <si>
+    <t>0.74 31.74  4.30</t>
+  </si>
+  <si>
+    <t>0.76 32.29  4.51</t>
+  </si>
+  <si>
+    <t>0.78 32.89  4.85</t>
+  </si>
+  <si>
+    <t>0.79 33.36  5.10</t>
+  </si>
+  <si>
+    <t>0.83 34.30  5.49 % N = 5</t>
+  </si>
+  <si>
+    <t>0.85 35.21  5.92</t>
+  </si>
+  <si>
+    <t>0.87 35.36  6.15</t>
+  </si>
+  <si>
+    <t>0.89 36.21  6.61</t>
+  </si>
+  <si>
+    <t>0.91 36.81  6.75</t>
+  </si>
+  <si>
+    <t>0.93 38.26  7.55 % N = 4</t>
+  </si>
+  <si>
+    <t>0.95 39.06  8.00</t>
+  </si>
+  <si>
+    <t>0.97 39.75  8.40</t>
+  </si>
+  <si>
+    <t>0.99 40.44  8.76</t>
+  </si>
+  <si>
+    <t>1.01 41.28  9.12</t>
+  </si>
+  <si>
+    <t>1.02 42.61  9.68</t>
+  </si>
+  <si>
+    <t>1.04 42.53  9.89</t>
+  </si>
+  <si>
+    <t>1.06 43.21 10.57</t>
+  </si>
+  <si>
+    <t>1.08 43.75 11.30</t>
+  </si>
+  <si>
+    <t>1.10 44.97 11.53</t>
+  </si>
+  <si>
+    <t>1.12 45.46 11.63</t>
+  </si>
+  <si>
+    <t>1.14 46.02 12.26</t>
+  </si>
+  <si>
+    <t>1.16 46.08 11.89</t>
+  </si>
+  <si>
+    <t>1.18 46.34 12.05</t>
+  </si>
+  <si>
+    <t>1.22 47.36 12.87</t>
+  </si>
+  <si>
+    <t>1.24 47.57 12.79</t>
+  </si>
+  <si>
+    <t>1.25 47.86 13.23</t>
+  </si>
+  <si>
+    <t>1.31 50.30 15.44 % N = 3</t>
+  </si>
+  <si>
+    <t>1.33 52.00 17.26 % N = 2</t>
+  </si>
+  <si>
+    <t>1.35 53.10 17.99</t>
+  </si>
+  <si>
+    <t>1.37 53.90 18.68</t>
+  </si>
+  <si>
+    <t>1.39 52.60 17.28 % N = 1</t>
+  </si>
+  <si>
+    <t>1.45 54.50 18.76</t>
+  </si>
+  <si>
+    <t>1.47 55.45 18.72</t>
+  </si>
+  <si>
+    <t>1.49 56.30 19.88</t>
+  </si>
+  <si>
+    <t>1.51 56.10 20.20</t>
+  </si>
+  <si>
+    <t>1.53 56.70 20.02</t>
+  </si>
+  <si>
+    <t>1.55 57.10 20.28</t>
+  </si>
+  <si>
+    <t>1.56 57.70 21.14</t>
+  </si>
+  <si>
+    <t>1.59 58.20 23.06</t>
+  </si>
+  <si>
+    <t>1.60 58.70 22.92</t>
+  </si>
+  <si>
+    <t>1.62 59.50 23.56</t>
+  </si>
+  <si>
+    <t>1.67 61.50 25.60</t>
+  </si>
+  <si>
+    <t>1.69 60.20 25.38</t>
+  </si>
+  <si>
+    <t>1.72 62.50 27.20</t>
+  </si>
+  <si>
+    <t>1.85 67.00 31.96</t>
+  </si>
+  <si>
+    <t>1.93 69.00 34.84];</t>
+  </si>
+  <si>
+    <t>Nind = find(tLW_Jone(:,1)&gt;=1.31); % find rows where there are three or fewer individuals --&gt; for setting low weights</t>
+  </si>
+  <si>
+    <t>tLW_Jone(:,1) = 365 * tLW_Jone(:,1); % convert yr to d</t>
+  </si>
+  <si>
+    <t>tLW_Jone(:,3) = 1e3 * tLW_Jone(:,3); % convert kg to g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data.tL_Jone = tLW_Jone(1:Nind(1)-1,1:2); % all data with four or more individiduals </t>
+  </si>
+  <si>
+    <t xml:space="preserve">units.tL_Jone   = {'d', 'cm'};  label.tL_Jone = {'time since birth', 'straight carapace length, Jones'};  </t>
+  </si>
+  <si>
+    <t>temp.tL_Jone    = C2K(24);  units.temp.tL_Jone = 'K'; label.temp.tL_Jone = 'temperature';</t>
+  </si>
+  <si>
+    <t>bibkey.tL_Jone = 'Jone2009';</t>
+  </si>
+  <si>
+    <t>comment.tL_Jone = ['data from Table 3.1, captive animals, fed with Pacific Ocean squid, Todarodes pacificus; '...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  '(mantle and tentacles only), vitamins (ReptaviteTM), and calcium (Rep-CalTM), '...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'blended with unflavored gelatin in hot water.'];</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data.tW_Jone = tLW_Jone(1:Nind(1)-1,[1 3]); </t>
+  </si>
+  <si>
+    <t xml:space="preserve">units.tW_Jone   = {'d', 'g'};  label.tW_Jone = {'time since birth', 'wet weight, Jones'};  </t>
+  </si>
+  <si>
+    <t>temp.tW_Jone    = C2K(24);  units.temp.tW_Jone = 'K'; label.temp.tW_Jone = 'temperature';</t>
+  </si>
+  <si>
+    <t>bibkey.tW_Jone = 'Jone2009';</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data.LW_Jone = tLW_Jone(1:Nind(1)-1,[2 3]); </t>
+  </si>
+  <si>
+    <t xml:space="preserve">units.LW_Jone   = {'cm', 'g'};  label.LW_Jone = {'straight carapace length', 'wet weight, Jones'};  </t>
+  </si>
+  <si>
+    <t>bibkey.LW_Jone = 'Jone2009';</t>
+  </si>
+  <si>
+    <t>% data below used for information only (only 3 or fewer individuals)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data.tL_Jone_i = tLW_Jone(Nind,1:2); % all data with four or more individiduals </t>
+  </si>
+  <si>
+    <t xml:space="preserve">units.tL_Jone_i   = {'d', 'cm'};  label.tL_Jone_i = {'time since birth', 'straight carapace length, Jones'};  </t>
+  </si>
+  <si>
+    <t>temp.tL_Jone_i    = C2K(24);  units.temp.tL_Jone_i = 'K'; label.temp.tL_Jone_i = 'temperature';</t>
+  </si>
+  <si>
+    <t>bibkey.tL_Jone_i = 'Jone2009';</t>
+  </si>
+  <si>
+    <t>comment.tL_Jone_i = '(informative) data from Table 3.1, where only 3 or fewer individuals- NOT used in fitting';</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data.tW_Jone_i = tLW_Jone(Nind,[1 3]); </t>
+  </si>
+  <si>
+    <t xml:space="preserve">units.tW_Jone_i   = {'d', 'g'};  label.tW_Jone_i = {'time since birth', 'wet weight, Jones'};  </t>
+  </si>
+  <si>
+    <t>temp.tW_Jone_i    = C2K(24);  units.temp.tW_Jone_i = 'K'; label.temp.tW_Jone_i = 'temperature';</t>
+  </si>
+  <si>
+    <t>bibkey.tW_Jone_i = 'Jone2009';</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data.LW_Jone_i = tLW_Jone(Nind,[2 3]); </t>
+  </si>
+  <si>
+    <t xml:space="preserve">units.LW_Jone_i   = {'cm', 'g'};  label.LW_Jone_i = {'straight carapace length', 'wet weight, Jones'};  </t>
+  </si>
+  <si>
+    <t>bibkey.LW_Jone_i = 'Jone2009';</t>
   </si>
 </sst>
 </file>
@@ -77,7 +501,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +511,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -114,13 +546,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -130,6 +559,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -151,7 +595,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -953,7 +1397,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1612,7 +2056,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3469,6 +3913,156 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>449037</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>68036</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>620487</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>96611</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{286B636F-AB6D-4CED-98BD-9A4D39DFC1D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15348858" y="6300107"/>
+          <a:ext cx="5614308" cy="4287611"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>612643</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>95572</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>603119</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>19372</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C671FF16-4E76-4863-93A4-E2240687BE64}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4626750" y="6327643"/>
+          <a:ext cx="5433333" cy="4359729"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>626571</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>95893</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>588472</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>143518</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3135CD4C-6EB2-4FFA-A6B0-F87A9973E9CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10083535" y="6327964"/>
+          <a:ext cx="5404758" cy="4306661"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3794,54 +4388,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M48"/>
+  <dimension ref="A1:AA60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="159" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="7"/>
+    <col min="1" max="1" width="8.875" style="6"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-    </row>
-    <row r="2" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="5" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+    </row>
+    <row r="2" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="6">
+    <row r="3" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
       <c r="B3" s="1">
@@ -3857,8 +4451,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="6">
+    <row r="4" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
       <c r="B4" s="1">
@@ -3874,8 +4468,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="6">
+    <row r="5" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
       <c r="B5" s="1">
@@ -3891,8 +4485,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="6">
+    <row r="6" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
       <c r="B6" s="1">
@@ -3908,8 +4502,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="6">
+    <row r="7" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
       <c r="B7" s="1">
@@ -3925,8 +4519,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="6">
+    <row r="8" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
       <c r="B8" s="1">
@@ -3942,8 +4536,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="6">
+    <row r="9" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
         <v>7</v>
       </c>
       <c r="B9" s="1">
@@ -3959,8 +4553,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="6">
+    <row r="10" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
         <v>8</v>
       </c>
       <c r="B10" s="1">
@@ -3976,8 +4570,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="6">
+    <row r="11" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
         <v>9</v>
       </c>
       <c r="B11" s="1">
@@ -3993,8 +4587,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="6">
+    <row r="12" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
         <v>10</v>
       </c>
       <c r="B12" s="1">
@@ -4010,8 +4604,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="6">
+    <row r="13" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
         <v>11</v>
       </c>
       <c r="B13" s="1">
@@ -4027,8 +4621,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="6">
+    <row r="14" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
         <v>12</v>
       </c>
       <c r="B14" s="1">
@@ -4044,8 +4638,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="6">
+    <row r="15" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
         <v>13</v>
       </c>
       <c r="B15" s="1">
@@ -4061,8 +4655,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="6">
+    <row r="16" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
         <v>14</v>
       </c>
       <c r="B16" s="1">
@@ -4078,8 +4672,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="6">
+    <row r="17" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
         <v>15</v>
       </c>
       <c r="B17" s="1">
@@ -4095,8 +4689,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="6">
+    <row r="18" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
         <v>16</v>
       </c>
       <c r="B18" s="1">
@@ -4112,8 +4706,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="6">
+    <row r="19" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
         <v>17</v>
       </c>
       <c r="B19" s="1">
@@ -4129,8 +4723,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="6">
+    <row r="20" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
         <v>18</v>
       </c>
       <c r="B20" s="1">
@@ -4146,8 +4740,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="6">
+    <row r="21" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
         <v>19</v>
       </c>
       <c r="B21" s="1">
@@ -4163,8 +4757,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="6">
+    <row r="22" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
         <v>20</v>
       </c>
       <c r="B22" s="1">
@@ -4180,8 +4774,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="7" t="s">
+    <row r="23" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="1">
@@ -4196,9 +4790,25 @@
       <c r="E23" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="7" t="s">
+      <c r="N23" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+      <c r="V23" s="11"/>
+      <c r="W23" s="11"/>
+      <c r="X23" s="11"/>
+      <c r="Y23" s="11"/>
+      <c r="Z23" s="11"/>
+      <c r="AA23" s="11"/>
+    </row>
+    <row r="24" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B24" s="1">
@@ -4213,9 +4823,23 @@
       <c r="E24" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="6">
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+      <c r="V24" s="11"/>
+      <c r="W24" s="11"/>
+      <c r="X24" s="11"/>
+      <c r="Y24" s="11"/>
+      <c r="Z24" s="11"/>
+      <c r="AA24" s="11"/>
+    </row>
+    <row r="25" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
         <v>1</v>
       </c>
       <c r="B25" s="1">
@@ -4230,9 +4854,23 @@
       <c r="E25" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="6">
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
+      <c r="V25" s="11"/>
+      <c r="W25" s="11"/>
+      <c r="X25" s="11"/>
+      <c r="Y25" s="11"/>
+      <c r="Z25" s="11"/>
+      <c r="AA25" s="11"/>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
         <v>2</v>
       </c>
       <c r="B26" s="1">
@@ -4247,9 +4885,23 @@
       <c r="E26" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="6">
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="11"/>
+      <c r="V26" s="11"/>
+      <c r="W26" s="11"/>
+      <c r="X26" s="11"/>
+      <c r="Y26" s="11"/>
+      <c r="Z26" s="11"/>
+      <c r="AA26" s="11"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A27" s="5">
         <v>3</v>
       </c>
       <c r="B27" s="1">
@@ -4264,9 +4916,23 @@
       <c r="E27" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="6">
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+      <c r="T27" s="11"/>
+      <c r="U27" s="11"/>
+      <c r="V27" s="11"/>
+      <c r="W27" s="11"/>
+      <c r="X27" s="11"/>
+      <c r="Y27" s="11"/>
+      <c r="Z27" s="11"/>
+      <c r="AA27" s="11"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
         <v>4</v>
       </c>
       <c r="B28" s="1">
@@ -4281,9 +4947,23 @@
       <c r="E28" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="6">
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="11"/>
+      <c r="V28" s="11"/>
+      <c r="W28" s="11"/>
+      <c r="X28" s="11"/>
+      <c r="Y28" s="11"/>
+      <c r="Z28" s="11"/>
+      <c r="AA28" s="11"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
         <v>5</v>
       </c>
       <c r="B29" s="1">
@@ -4298,9 +4978,23 @@
       <c r="E29" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="6">
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11"/>
+      <c r="T29" s="11"/>
+      <c r="U29" s="11"/>
+      <c r="V29" s="11"/>
+      <c r="W29" s="11"/>
+      <c r="X29" s="11"/>
+      <c r="Y29" s="11"/>
+      <c r="Z29" s="11"/>
+      <c r="AA29" s="11"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
         <v>6</v>
       </c>
       <c r="B30" s="1">
@@ -4315,9 +5009,23 @@
       <c r="E30" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="6">
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
+      <c r="T30" s="11"/>
+      <c r="U30" s="11"/>
+      <c r="V30" s="11"/>
+      <c r="W30" s="11"/>
+      <c r="X30" s="11"/>
+      <c r="Y30" s="11"/>
+      <c r="Z30" s="11"/>
+      <c r="AA30" s="11"/>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
         <v>7</v>
       </c>
       <c r="B31" s="1">
@@ -4332,9 +5040,23 @@
       <c r="E31" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32" s="6">
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
+      <c r="T31" s="11"/>
+      <c r="U31" s="11"/>
+      <c r="V31" s="11"/>
+      <c r="W31" s="11"/>
+      <c r="X31" s="11"/>
+      <c r="Y31" s="11"/>
+      <c r="Z31" s="11"/>
+      <c r="AA31" s="11"/>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
         <v>8</v>
       </c>
       <c r="B32" s="1">
@@ -4349,9 +5071,23 @@
       <c r="E32" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="6">
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
+      <c r="T32" s="11"/>
+      <c r="U32" s="11"/>
+      <c r="V32" s="11"/>
+      <c r="W32" s="11"/>
+      <c r="X32" s="11"/>
+      <c r="Y32" s="11"/>
+      <c r="Z32" s="11"/>
+      <c r="AA32" s="11"/>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
         <v>9</v>
       </c>
       <c r="B33" s="1">
@@ -4366,9 +5102,23 @@
       <c r="E33" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" s="6">
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
+      <c r="S33" s="11"/>
+      <c r="T33" s="11"/>
+      <c r="U33" s="11"/>
+      <c r="V33" s="11"/>
+      <c r="W33" s="11"/>
+      <c r="X33" s="11"/>
+      <c r="Y33" s="11"/>
+      <c r="Z33" s="11"/>
+      <c r="AA33" s="11"/>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
         <v>10</v>
       </c>
       <c r="B34" s="1">
@@ -4384,8 +5134,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="6">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A35" s="5">
         <v>11</v>
       </c>
       <c r="B35" s="1">
@@ -4401,8 +5151,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="6">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A36" s="5">
         <v>12</v>
       </c>
       <c r="B36" s="1">
@@ -4418,8 +5168,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="6">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A37" s="5">
         <v>13</v>
       </c>
       <c r="B37" s="1">
@@ -4435,8 +5185,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="6">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
         <v>14</v>
       </c>
       <c r="B38" s="1">
@@ -4452,8 +5202,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="7" t="s">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B39" s="1">
@@ -4469,8 +5219,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" s="7" t="s">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B40" s="1">
@@ -4486,8 +5236,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="6">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A41" s="5">
         <v>1</v>
       </c>
       <c r="B41" s="1">
@@ -4503,8 +5253,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="6">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A42" s="5">
         <v>2</v>
       </c>
       <c r="B42" s="1">
@@ -4520,8 +5270,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="6">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A43" s="5">
         <v>3</v>
       </c>
       <c r="B43" s="1">
@@ -4537,8 +5287,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="6">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A44" s="5">
         <v>4</v>
       </c>
       <c r="B44" s="1">
@@ -4554,8 +5304,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="6">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A45" s="5">
         <v>5</v>
       </c>
       <c r="B45" s="1">
@@ -4571,8 +5321,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="6">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A46" s="5">
         <v>6</v>
       </c>
       <c r="B46" s="1">
@@ -4588,8 +5338,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="6">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A47" s="5">
         <v>7</v>
       </c>
       <c r="B47" s="1">
@@ -4605,8 +5355,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48" s="6">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A48" s="5">
         <v>8</v>
       </c>
       <c r="B48" s="1">
@@ -4622,17 +5372,824 @@
         <v>5</v>
       </c>
     </row>
+    <row r="49" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A49" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B49" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="9">
+        <v>34182</v>
+      </c>
+      <c r="B50" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50" s="1">
+        <v>39</v>
+      </c>
+      <c r="D50">
+        <v>7</v>
+      </c>
+      <c r="E50" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="9">
+        <v>12663</v>
+      </c>
+      <c r="B51" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="D51">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="E51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="10">
+        <v>45540</v>
+      </c>
+      <c r="B52" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52" s="1">
+        <v>10.4</v>
+      </c>
+      <c r="D52">
+        <v>0.19</v>
+      </c>
+      <c r="E52" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="10">
+        <v>45357</v>
+      </c>
+      <c r="B53" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53" s="1">
+        <v>25</v>
+      </c>
+      <c r="D53">
+        <v>3.1</v>
+      </c>
+      <c r="E53" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="9">
+        <v>35886</v>
+      </c>
+      <c r="B54" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" s="1">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="D54">
+        <v>44.5</v>
+      </c>
+      <c r="E54" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="9">
+        <v>36251</v>
+      </c>
+      <c r="B55" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55" s="1">
+        <v>85.3</v>
+      </c>
+      <c r="D55">
+        <v>74.099999999999994</v>
+      </c>
+      <c r="E55" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="10">
+        <v>45388</v>
+      </c>
+      <c r="B56" t="s">
+        <v>27</v>
+      </c>
+      <c r="C56" s="1">
+        <v>70</v>
+      </c>
+      <c r="D56">
+        <v>35.450000000000003</v>
+      </c>
+      <c r="E56" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="10">
+        <v>45479</v>
+      </c>
+      <c r="B57" t="s">
+        <v>27</v>
+      </c>
+      <c r="C57" s="1">
+        <v>67.5</v>
+      </c>
+      <c r="D57">
+        <v>33.6</v>
+      </c>
+      <c r="E57" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="10">
+        <v>45475</v>
+      </c>
+      <c r="B58" t="s">
+        <v>28</v>
+      </c>
+      <c r="C58" s="1">
+        <v>20</v>
+      </c>
+      <c r="D58">
+        <v>1.85</v>
+      </c>
+      <c r="E58" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="6">
+        <v>1983</v>
+      </c>
+      <c r="B59" t="s">
+        <v>28</v>
+      </c>
+      <c r="C59" s="1">
+        <v>31</v>
+      </c>
+      <c r="D59">
+        <v>3.3</v>
+      </c>
+      <c r="E59" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B60" t="s">
+        <v>26</v>
+      </c>
+      <c r="C60" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="D60">
+        <v>0.17</v>
+      </c>
+      <c r="E60" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:F48" xr:uid="{628915EA-6431-3E4F-B108-7FB921E8B197}"/>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:M1"/>
+    <mergeCell ref="N23:AA33"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D12AEE23-EBD3-4BD8-A2EA-CE68C5958BC4}">
+  <dimension ref="A1:A122"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="E97" sqref="E97"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>147</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>